<commit_message>
including most up to date Clomeleon data as xl file
</commit_message>
<xml_diff>
--- a/SPNratios_longformat.xlsx
+++ b/SPNratios_longformat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\april\Documents\WennerLAb\Imaging\Summary\JNM_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A47D576B-4E1B-421D-A9F4-264108F98AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD203D6C-B774-4D5E-91D0-45273F989BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{65F4048B-F060-42FE-9E04-1C074A7FC4BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{65F4048B-F060-42FE-9E04-1C074A7FC4BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -419,17 +419,17 @@
   <dimension ref="A1:E146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96:D146"/>
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -446,7 +446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -464,7 +464,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -481,7 +481,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -498,7 +498,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -515,7 +515,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -532,7 +532,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -549,7 +549,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -566,7 +566,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -583,7 +583,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -600,7 +600,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -617,7 +617,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -634,7 +634,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -651,7 +651,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -668,7 +668,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -685,7 +685,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -702,7 +702,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -719,7 +719,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -736,7 +736,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -753,7 +753,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -770,7 +770,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -787,7 +787,7 @@
         <v>32422</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -804,7 +804,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -821,7 +821,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -838,7 +838,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -855,7 +855,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -872,7 +872,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -889,7 +889,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -906,7 +906,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -923,7 +923,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -940,7 +940,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -957,7 +957,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -974,7 +974,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -991,7 +991,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>61622</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>62222</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>3</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>3</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>3</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>3</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>3</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>3</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>70522</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>70822</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>70822</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>3</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>70822</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>70822</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>3</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>70822</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>70822</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>3</v>
       </c>
@@ -2039,13 +2039,13 @@
         <v>82.566999999999993</v>
       </c>
       <c r="D95">
-        <v>1.8359998546634857</v>
+        <v>1.8359998546634899</v>
       </c>
       <c r="E95">
         <v>70822</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>4</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>51022</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>4</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>51022</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>4</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>51022</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>4</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>51022</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>4</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>51022</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>4</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>51022</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>51022</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>4</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>51022</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>4</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>60622</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>4</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>60622</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>4</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>60622</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>4</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>60622</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>4</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>60622</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>4</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>60622</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>4</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>60722</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>4</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>60722</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>4</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>60722</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>4</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>60722</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>4</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>4</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>4</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>4</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>4</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>4</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>4</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>4</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>4</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>4</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>4</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>4</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>4</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>62322</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>4</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>4</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>4</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>4</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>4</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>4</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>4</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>4</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>4</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>4</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>4</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>4</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>4</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>70122</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>4</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>71622</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>4</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>71622</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>4</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>71622</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>4</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>71622</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>4</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>71622</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>4</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>71622</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>4</v>
       </c>

</xml_diff>